<commit_message>
Updated department website on 12th september 2025
</commit_message>
<xml_diff>
--- a/public/research_excel/ongoing_projects.xlsx
+++ b/public/research_excel/ongoing_projects.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web_page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S417\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FA10FA3-5EB2-42FC-9B06-DA416BE8065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7AF392-4A11-44DE-8141-0A5B64EEA1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E46560EE-D38D-43DB-9F03-BD715BDEEA66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>Year</t>
   </si>
@@ -423,6 +426,27 @@
   </si>
   <si>
     <t>Single-molecule imaging of yeast sirtuin Sir2 to understand its trafficking and target-search mechanism for transcription silencing.</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>DST</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>IIT Hyderabad</t>
+  </si>
+  <si>
+    <t>Other sources</t>
+  </si>
+  <si>
+    <t>MOE</t>
+  </si>
+  <si>
+    <t>International</t>
   </si>
 </sst>
 </file>
@@ -794,15 +818,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94B2841-D398-4EA5-B6D1-3FCBD21A8929}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G35"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="105" customWidth="1"/>
+    <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -824,8 +852,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -844,8 +875,11 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -864,8 +898,11 @@
       <c r="G3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -884,8 +921,11 @@
       <c r="G4">
         <v>54.59</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -904,8 +944,11 @@
       <c r="G5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -924,8 +967,11 @@
       <c r="G6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -944,8 +990,11 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -964,8 +1013,11 @@
       <c r="G8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -984,8 +1036,11 @@
       <c r="G9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -1004,8 +1059,11 @@
       <c r="G10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -1024,8 +1082,11 @@
       <c r="G11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -1041,8 +1102,11 @@
       <c r="G12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -1061,8 +1125,11 @@
       <c r="G13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -1081,8 +1148,11 @@
       <c r="G14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2022</v>
       </c>
@@ -1101,8 +1171,11 @@
       <c r="G15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -1121,8 +1194,11 @@
       <c r="G16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2022</v>
       </c>
@@ -1141,8 +1217,11 @@
       <c r="G17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2022</v>
       </c>
@@ -1161,8 +1240,11 @@
       <c r="G18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2022</v>
       </c>
@@ -1181,8 +1263,11 @@
       <c r="G19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2022</v>
       </c>
@@ -1201,8 +1286,11 @@
       <c r="G20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2023</v>
       </c>
@@ -1221,8 +1309,11 @@
       <c r="G21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2023</v>
       </c>
@@ -1241,8 +1332,11 @@
       <c r="G22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2023</v>
       </c>
@@ -1261,8 +1355,11 @@
       <c r="G23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2023</v>
       </c>
@@ -1281,8 +1378,11 @@
       <c r="G24" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2023</v>
       </c>
@@ -1301,8 +1401,11 @@
       <c r="G25" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2023</v>
       </c>
@@ -1321,8 +1424,11 @@
       <c r="G26" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2023</v>
       </c>
@@ -1341,8 +1447,11 @@
       <c r="G27" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2023</v>
       </c>
@@ -1361,8 +1470,11 @@
       <c r="G28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2023</v>
       </c>
@@ -1381,8 +1493,11 @@
       <c r="G29" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2023</v>
       </c>
@@ -1401,8 +1516,11 @@
       <c r="G30" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2023</v>
       </c>
@@ -1421,8 +1539,11 @@
       <c r="G31" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2023</v>
       </c>
@@ -1441,8 +1562,11 @@
       <c r="G32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2024</v>
       </c>
@@ -1458,8 +1582,11 @@
       <c r="F33" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2024</v>
       </c>
@@ -1478,8 +1605,11 @@
       <c r="G34" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2025</v>
       </c>
@@ -1492,8 +1622,12 @@
       <c r="E35" t="s">
         <v>128</v>
       </c>
+      <c r="H35" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D35" xr:uid="{F94B2841-D398-4EA5-B6D1-3FCBD21A8929}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>